<commit_message>
MAJ collecteurs (prix + chemins)
</commit_message>
<xml_diff>
--- a/prix/collecteur.xlsx
+++ b/prix/collecteur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\raccords-plomberie\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6349EDE8-466D-4F7B-A65C-D36D7EA48DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD9934A-C2E2-472B-AAEF-97949AC15704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC89CC73-BE36-4334-9D51-D90570969AD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
   <si>
     <t>43120560</t>
   </si>
@@ -218,36 +218,12 @@
     <t>4/4</t>
   </si>
   <si>
-    <t>collecteur/collecteur-2-bleu.png</t>
-  </si>
-  <si>
     <t>collecteur/collecteur-2-rouge.png</t>
   </si>
   <si>
-    <t>collecteur/collecteur-3-bleu.png</t>
-  </si>
-  <si>
     <t>collecteur/collecteur-3-rouge.png</t>
   </si>
   <si>
-    <t>collecteur/collecteur-4-bleu.png</t>
-  </si>
-  <si>
-    <t>collecteur/collecteur-4-rouge.png</t>
-  </si>
-  <si>
-    <t>collecteur/collecteur-5-bleu.png</t>
-  </si>
-  <si>
-    <t>collecteur/collecteur-5-rouge.png</t>
-  </si>
-  <si>
-    <t>collecteur/collecteur-6-bleu.png</t>
-  </si>
-  <si>
-    <t>collecteur/collecteur-6-rouge.png</t>
-  </si>
-  <si>
     <t>3/4-2</t>
   </si>
   <si>
@@ -273,6 +249,33 @@
   </si>
   <si>
     <t>4/4-5</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-4-rouge.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-5-rouge.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-6-rouge.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-2-bleu.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-3-bleu.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-4-bleu.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-5-bleu.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-6-bleu.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-2-rouge.png</t>
   </si>
 </sst>
 </file>
@@ -683,13 +686,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5862B2-EBB0-4D15-9659-D132FB8D0373}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.21875" style="6" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
@@ -730,13 +733,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D2" s="8">
         <v>19.78</v>
@@ -747,13 +750,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D3" s="8">
         <v>26.73</v>
@@ -764,13 +767,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D4" s="8">
         <v>35.69</v>
@@ -781,13 +784,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D5" s="8">
         <v>40.56</v>
@@ -798,13 +801,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D6" s="8">
         <v>47.7</v>
@@ -815,13 +818,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D7" s="8">
         <v>17.77</v>
@@ -832,13 +835,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D8" s="8">
         <v>25.13</v>
@@ -849,13 +852,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D9" s="8">
         <v>33.54</v>
@@ -866,13 +869,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D10" s="8">
         <v>36.700000000000003</v>
@@ -883,13 +886,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D11" s="8">
         <v>47.7</v>
@@ -986,13 +989,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D19" s="8">
         <v>19.59</v>
@@ -1003,13 +1006,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D20" s="8">
         <v>19.59</v>
@@ -1020,13 +1023,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D21" s="8">
         <v>42.78</v>
@@ -1037,13 +1040,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D22" s="8">
         <v>42.78</v>

</xml_diff>

<commit_message>
Fix paths collecteurs + tailles 3/4-2.. et 4/4
</commit_message>
<xml_diff>
--- a/prix/collecteur.xlsx
+++ b/prix/collecteur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\raccords-plomberie\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD9934A-C2E2-472B-AAEF-97949AC15704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC86DBF9-5B7B-47D1-B692-5AC3AB65CD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC89CC73-BE36-4334-9D51-D90570969AD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t>43120560</t>
   </si>
@@ -215,15 +215,6 @@
     <t>denomination</t>
   </si>
   <si>
-    <t>4/4</t>
-  </si>
-  <si>
-    <t>collecteur/collecteur-2-rouge.png</t>
-  </si>
-  <si>
-    <t>collecteur/collecteur-3-rouge.png</t>
-  </si>
-  <si>
     <t>3/4-2</t>
   </si>
   <si>
@@ -242,12 +233,6 @@
     <t>4/4-2</t>
   </si>
   <si>
-    <t>4/4-3</t>
-  </si>
-  <si>
-    <t>4/4-4</t>
-  </si>
-  <si>
     <t>4/4-5</t>
   </si>
   <si>
@@ -276,6 +261,9 @@
   </si>
   <si>
     <t>collecteurs/collecteur-2-rouge.png</t>
+  </si>
+  <si>
+    <t>collecteurs/collecteur-3-rouge.png</t>
   </si>
 </sst>
 </file>
@@ -686,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5862B2-EBB0-4D15-9659-D132FB8D0373}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,13 +721,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" s="8">
         <v>19.78</v>
@@ -750,13 +738,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" s="8">
         <v>26.73</v>
@@ -767,13 +755,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D4" s="8">
         <v>35.69</v>
@@ -784,13 +772,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D5" s="8">
         <v>40.56</v>
@@ -801,13 +789,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D6" s="8">
         <v>47.7</v>
@@ -818,13 +806,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" s="8">
         <v>17.77</v>
@@ -835,13 +823,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="8">
         <v>25.13</v>
@@ -852,13 +840,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9" s="8">
         <v>33.54</v>
@@ -869,13 +857,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10" s="8">
         <v>36.700000000000003</v>
@@ -886,13 +874,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D11" s="8">
         <v>47.7</v>
@@ -977,9 +965,7 @@
       <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="8">
         <v>5.17</v>
       </c>
@@ -989,13 +975,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" s="8">
         <v>19.59</v>
@@ -1006,13 +992,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" s="8">
         <v>19.59</v>
@@ -1023,13 +1009,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D21" s="8">
         <v>42.78</v>
@@ -1040,13 +1026,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D22" s="8">
         <v>42.78</v>

</xml_diff>